<commit_message>
fix: Corriger formules Excel =TRUE()/=FALSE() → valeurs booléennes
49 formules Excel corrigées:
- =TRUE() → True
- =FALSE() → False

Les formules n'étaient pas évaluées par pandas lors de la lecture,
causant des erreurs de validation booléenne dans Ansible.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/aci_fabric_config.xlsx
+++ b/aci_fabric_config.xlsx
@@ -4940,9 +4940,8 @@
           <t>CDP_Enabled</t>
         </is>
       </c>
-      <c r="B2" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="B2" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="C2" s="8" t="inlineStr">
         <is>
@@ -4956,9 +4955,8 @@
           <t>CDP_Disabled</t>
         </is>
       </c>
-      <c r="B3" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="B3" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="C3" s="8" t="inlineStr">
         <is>
@@ -5158,13 +5156,11 @@
           <t>LLDP_Enabled</t>
         </is>
       </c>
-      <c r="B2" s="8">
-        <f>TRUE()</f>
-        <v/>
-      </c>
-      <c r="C2" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="B2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
@@ -5178,13 +5174,11 @@
           <t>LLDP_RxOnly</t>
         </is>
       </c>
-      <c r="B3" s="8">
-        <f>TRUE()</f>
-        <v/>
-      </c>
-      <c r="C3" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="B3" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
@@ -5198,13 +5192,11 @@
           <t>LLDP_Disabled</t>
         </is>
       </c>
-      <c r="B4" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="C4" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="B4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
@@ -5286,9 +5278,8 @@
           <t>MCP_Strict</t>
         </is>
       </c>
-      <c r="B2" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="B2" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="C2" s="8" t="inlineStr">
         <is>
@@ -5322,9 +5313,8 @@
           <t>MCP_NonStrict</t>
         </is>
       </c>
-      <c r="B3" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="B3" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="C3" s="8" t="inlineStr">
         <is>
@@ -5442,25 +5432,20 @@
       <c r="D2" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="8">
-        <f>TRUE()</f>
-        <v/>
-      </c>
-      <c r="F2" s="8">
-        <f>TRUE()</f>
-        <v/>
-      </c>
-      <c r="G2" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="H2" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="I2" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="E2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="J2" s="8" t="inlineStr">
         <is>
@@ -5485,25 +5470,20 @@
       <c r="D3" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="F3" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="G3" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="H3" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="I3" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="E3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="J3" s="8" t="inlineStr">
         <is>
@@ -5560,13 +5540,11 @@
           <t>STP_BPDUGuard</t>
         </is>
       </c>
-      <c r="B2" s="8">
-        <f>TRUE()</f>
-        <v/>
-      </c>
-      <c r="C2" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="B2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
@@ -5580,13 +5558,11 @@
           <t>STP_BPDUFilter</t>
         </is>
       </c>
-      <c r="B3" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="C3" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="B3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
@@ -5600,13 +5576,11 @@
           <t>STP_Default</t>
         </is>
       </c>
-      <c r="B4" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="C4" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="B4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
@@ -7349,9 +7323,8 @@
           <t>10.10.1.101</t>
         </is>
       </c>
-      <c r="G2" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="G2" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="6">
@@ -7381,9 +7354,8 @@
           <t>10.10.1.102</t>
         </is>
       </c>
-      <c r="G3" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="G3" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="6">
@@ -7413,9 +7385,8 @@
           <t>10.1.1.101</t>
         </is>
       </c>
-      <c r="G4" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="G4" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7822,13 +7793,11 @@
           <t>Prod_VRF</t>
         </is>
       </c>
-      <c r="D2" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="E2" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="D2" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="F2" s="8" t="inlineStr">
         <is>
@@ -7857,13 +7826,11 @@
           <t>Prod_VRF</t>
         </is>
       </c>
-      <c r="D3" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="E3" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="D3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="F3" s="8" t="inlineStr">
         <is>
@@ -7892,13 +7859,11 @@
           <t>Prod_VRF</t>
         </is>
       </c>
-      <c r="D4" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="E4" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="D4" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
@@ -7927,13 +7892,11 @@
           <t>Dev_VRF</t>
         </is>
       </c>
-      <c r="D5" s="8">
-        <f>TRUE()</f>
-        <v/>
-      </c>
-      <c r="E5" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="D5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="F5" s="8" t="inlineStr">
         <is>
@@ -7962,13 +7925,11 @@
           <t>Dev_VRF</t>
         </is>
       </c>
-      <c r="D6" s="8">
-        <f>TRUE()</f>
-        <v/>
-      </c>
-      <c r="E6" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="D6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="F6" s="8" t="inlineStr">
         <is>
@@ -7997,13 +7958,11 @@
           <t>DMZ_VRF</t>
         </is>
       </c>
-      <c r="D7" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="E7" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="D7" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="F7" s="8" t="inlineStr">
         <is>
@@ -8032,13 +7991,11 @@
           <t>DMZ_VRF</t>
         </is>
       </c>
-      <c r="D8" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="E8" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="D8" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="F8" s="8" t="inlineStr">
         <is>
@@ -8067,13 +8024,11 @@
           <t>Mgmt_VRF</t>
         </is>
       </c>
-      <c r="D9" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="E9" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="D9" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="F9" s="8" t="inlineStr">
         <is>
@@ -8102,13 +8057,11 @@
           <t>Prod_VRF</t>
         </is>
       </c>
-      <c r="D10" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="E10" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="D10" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="F10" s="8" t="inlineStr">
         <is>
@@ -8137,13 +8090,11 @@
           <t>Prod_VRF</t>
         </is>
       </c>
-      <c r="D11" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="E11" s="8">
-        <f>TRUE()</f>
-        <v/>
+      <c r="D11" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="F11" s="8" t="inlineStr">
         <is>
@@ -8172,13 +8123,11 @@
           <t>Prod_VRF</t>
         </is>
       </c>
-      <c r="D12" s="8">
-        <f>FALSE()</f>
-        <v/>
-      </c>
-      <c r="E12" s="8">
-        <f>FALSE()</f>
-        <v/>
+      <c r="D12" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="F12" s="8" t="inlineStr">
         <is>
@@ -10564,22 +10513,22 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>Production</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>Test_Match_Rule</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="8" t="inlineStr">
         <is>
           <t>Match rule pour Route Control</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" s="8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10629,22 +10578,22 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>Production</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>Test_Match_Rule</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="8" t="inlineStr">
         <is>
           <t>11.11.11.11/24</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" s="8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10694,22 +10643,22 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>Production</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>Test_L3Out_Prod_Standard</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="8" t="inlineStr">
         <is>
           <t>Test_RouteControl_Profile</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" s="8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10771,32 +10720,32 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>Production</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>Test_L3Out_Prod_Standard</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="8" t="inlineStr">
         <is>
           <t>Test_RouteControl_Profile</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="8" t="inlineStr">
         <is>
           <t>Test_RouteControl_Context</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="8" t="inlineStr">
         <is>
           <t>Test_Match_Rule</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" s="8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>